<commit_message>
Replaced NaNs with NAs
</commit_message>
<xml_diff>
--- a/mm.06pho.xlsx
+++ b/mm.06pho.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ananya\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ananya\Documents\GitHub\GurvichFig1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81ACE39C-DA94-4F86-958B-EA5B80F965C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266B8327-8D4D-4698-A12D-4CF5E58D5177}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="1905" windowWidth="21600" windowHeight="11835" xr2:uid="{A53B43BB-18F4-4BED-8DDC-F97EF3C48256}"/>
+    <workbookView xWindow="7200" yWindow="1980" windowWidth="21600" windowHeight="11835" xr2:uid="{A53B43BB-18F4-4BED-8DDC-F97EF3C48256}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
-    <t>NaN</t>
-  </si>
-  <si>
     <t>_1</t>
   </si>
   <si>
@@ -60,6 +57,9 @@
   </si>
   <si>
     <t>_24.67</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -422,28 +422,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -968,7 +968,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B22">
         <v>0.24091417782028299</v>
@@ -977,7 +977,7 @@
         <v>0.30380951150704999</v>
       </c>
       <c r="D22" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E22">
         <v>1.3592128765812601</v>

</xml_diff>